<commit_message>
Update results 10mm pinned
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D26508E-022B-4C8E-8019-B752BF612D82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454FD531-9BC8-44F3-ABA9-2312C48D8D74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-26745" yWindow="1230" windowWidth="21600" windowHeight="11385" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Test #</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Flexsor Test 10mm</t>
+  </si>
+  <si>
+    <t>*Fish scale seems to be +/- 1 N</t>
   </si>
 </sst>
 </file>
@@ -597,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
-  <dimension ref="A1:Q15"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,7 +628,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>520</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -634,7 +637,7 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>431.6</v>
+        <v>381.8</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -700,7 +703,31 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>33.299999999999997</v>
+        <v>22.3</v>
+      </c>
+      <c r="D6">
+        <v>21.6</v>
+      </c>
+      <c r="E6">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="F6">
+        <v>13.7</v>
+      </c>
+      <c r="G6">
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="H6">
+        <v>7.8</v>
+      </c>
+      <c r="I6">
+        <v>5.9</v>
+      </c>
+      <c r="J6">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -708,7 +735,31 @@
         <v>2</v>
       </c>
       <c r="C7">
-        <v>75</v>
+        <v>102</v>
+      </c>
+      <c r="D7">
+        <v>100</v>
+      </c>
+      <c r="E7">
+        <v>81.5</v>
+      </c>
+      <c r="F7">
+        <v>66</v>
+      </c>
+      <c r="G7">
+        <v>47</v>
+      </c>
+      <c r="H7">
+        <v>35</v>
+      </c>
+      <c r="I7">
+        <v>17</v>
+      </c>
+      <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -718,23 +769,38 @@
       <c r="B8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="2">
-        <v>40.5</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="C8" s="4">
+        <v>68.099999999999994</v>
+      </c>
+      <c r="D8" s="4">
+        <v>67.900000000000006</v>
+      </c>
+      <c r="E8" s="4">
+        <v>68.599999999999994</v>
+      </c>
+      <c r="F8" s="4">
+        <v>70.8</v>
+      </c>
+      <c r="G8" s="4">
+        <v>70.8</v>
+      </c>
+      <c r="H8" s="4">
+        <v>72.3</v>
+      </c>
+      <c r="I8" s="4">
+        <v>74.900000000000006</v>
+      </c>
+      <c r="J8" s="4">
+        <v>75.400000000000006</v>
+      </c>
+      <c r="K8" s="4">
+        <v>77.5</v>
+      </c>
       <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-      <c r="Q8" s="4"/>
     </row>
     <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="14"/>
@@ -755,30 +821,44 @@
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
-      <c r="Q9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C10">
-        <v>435</v>
-      </c>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="16"/>
-      <c r="G10" s="16"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="16"/>
-      <c r="J10" s="16"/>
-      <c r="K10" s="16"/>
+      <c r="C10" s="16">
+        <v>430</v>
+      </c>
+      <c r="D10" s="16">
+        <v>430</v>
+      </c>
+      <c r="E10" s="16">
+        <v>420</v>
+      </c>
+      <c r="F10" s="16">
+        <v>415</v>
+      </c>
+      <c r="G10" s="16">
+        <v>410</v>
+      </c>
+      <c r="H10" s="16">
+        <v>401</v>
+      </c>
+      <c r="I10" s="16">
+        <v>390</v>
+      </c>
+      <c r="J10" s="16">
+        <v>388</v>
+      </c>
+      <c r="K10" s="16">
+        <v>385</v>
+      </c>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-      <c r="Q10" s="1"/>
     </row>
     <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
@@ -835,9 +915,6 @@
       <c r="P12" s="16">
         <v>268.06</v>
       </c>
-      <c r="Q12" s="16">
-        <v>268.06</v>
-      </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A13" s="14"/>
@@ -847,14 +924,30 @@
       <c r="C13" s="16">
         <v>30</v>
       </c>
-      <c r="D13" s="16"/>
-      <c r="E13" s="16"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="16"/>
-      <c r="H13" s="16"/>
-      <c r="I13" s="16"/>
-      <c r="J13" s="16"/>
-      <c r="K13" s="16"/>
+      <c r="D13" s="16">
+        <v>30</v>
+      </c>
+      <c r="E13" s="16">
+        <v>30</v>
+      </c>
+      <c r="F13" s="16">
+        <v>30</v>
+      </c>
+      <c r="G13" s="16">
+        <v>34</v>
+      </c>
+      <c r="H13" s="16">
+        <v>35</v>
+      </c>
+      <c r="I13" s="16">
+        <v>45</v>
+      </c>
+      <c r="J13" s="16">
+        <v>50</v>
+      </c>
+      <c r="K13" s="16">
+        <v>55</v>
+      </c>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -867,43 +960,43 @@
         <v>6</v>
       </c>
       <c r="C15">
-        <f>C6*SIN(RADIANS(C8))*C12/1000</f>
-        <v>5.7972317597184544</v>
+        <f t="shared" ref="C15:J15" si="0">C6*COS(RADIANS(C9-3.05))*C12/1000</f>
+        <v>5.9692704311431557</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="D15:K15" si="0">D6*COS(RADIANS(D9-3.05))*D12/1000</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>5.7818942292687066</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4.9788533640924975</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.6672199509713548</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.6232668262422836</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>2.0879062494581437</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5793137015132115</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.3116334131211418</v>
       </c>
       <c r="K15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="K15:P15" si="1">K6*COS(RADIANS(K9-2.83))*K12/1000</f>
         <v>0</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:Q15" si="1">L6*COS(RADIANS(L9-2.83))*L12/1000</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15">
@@ -922,9 +1015,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q15">
-        <f t="shared" si="1"/>
-        <v>0</v>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -938,7 +1032,7 @@
   <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -963,7 +1057,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>415</v>
+        <v>460</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -972,7 +1066,7 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>344.45</v>
+        <v>381.8</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -1030,34 +1124,7 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>23.454999999999998</v>
-      </c>
-      <c r="D6">
-        <v>23.064</v>
-      </c>
-      <c r="E6">
-        <v>21.006</v>
-      </c>
-      <c r="F6">
-        <v>15.817</v>
-      </c>
-      <c r="G6">
-        <v>11.64</v>
-      </c>
-      <c r="H6">
-        <v>7.8520000000000003</v>
-      </c>
-      <c r="I6">
-        <v>7.0689000000000002</v>
-      </c>
-      <c r="J6">
-        <v>4.274</v>
-      </c>
-      <c r="K6">
-        <v>2.855</v>
-      </c>
-      <c r="L6">
-        <v>1.2350000000000001</v>
+        <v>33.299999999999997</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -1067,33 +1134,6 @@
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="D7">
-        <v>11</v>
-      </c>
-      <c r="E7">
-        <v>16</v>
-      </c>
-      <c r="F7">
-        <v>26.5</v>
-      </c>
-      <c r="G7">
-        <v>40</v>
-      </c>
-      <c r="H7">
-        <v>49.5</v>
-      </c>
-      <c r="I7">
-        <v>54.5</v>
-      </c>
-      <c r="J7">
-        <v>61</v>
-      </c>
-      <c r="K7">
-        <v>63.5</v>
-      </c>
-      <c r="L7">
-        <v>81</v>
-      </c>
     </row>
     <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
@@ -1105,33 +1145,15 @@
       <c r="C8" s="2">
         <v>6</v>
       </c>
-      <c r="D8" s="4">
-        <v>24</v>
-      </c>
-      <c r="E8" s="4">
-        <v>20</v>
-      </c>
-      <c r="F8" s="4">
-        <v>25.5</v>
-      </c>
-      <c r="G8" s="4">
-        <v>26.7</v>
-      </c>
-      <c r="H8" s="4">
-        <v>26.7</v>
-      </c>
-      <c r="I8" s="4">
-        <v>32.700000000000003</v>
-      </c>
-      <c r="J8" s="4">
-        <v>29.75</v>
-      </c>
-      <c r="K8" s="4">
-        <v>28.15</v>
-      </c>
-      <c r="L8" s="4">
-        <v>37.9</v>
-      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4"/>
+      <c r="L8" s="4"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1143,36 +1165,16 @@
       <c r="B9" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="16">
-        <v>23</v>
-      </c>
-      <c r="D9" s="16">
-        <v>23</v>
-      </c>
-      <c r="E9" s="16">
-        <v>21</v>
-      </c>
-      <c r="F9" s="16">
-        <v>23</v>
-      </c>
-      <c r="G9" s="16">
-        <v>28</v>
-      </c>
-      <c r="H9" s="16">
-        <v>28</v>
-      </c>
-      <c r="I9" s="16">
-        <v>29.5</v>
-      </c>
-      <c r="J9" s="16">
-        <v>34</v>
-      </c>
-      <c r="K9" s="16">
-        <v>34</v>
-      </c>
-      <c r="L9" s="16">
-        <v>41</v>
-      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="16"/>
+      <c r="K9" s="16"/>
+      <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -1187,33 +1189,15 @@
       <c r="C10">
         <v>397</v>
       </c>
-      <c r="D10" s="16">
-        <v>390</v>
-      </c>
-      <c r="E10" s="16">
-        <v>387</v>
-      </c>
-      <c r="F10" s="16">
-        <v>380</v>
-      </c>
-      <c r="G10" s="16">
-        <v>375</v>
-      </c>
-      <c r="H10" s="16">
-        <v>371</v>
-      </c>
-      <c r="I10" s="16">
-        <v>367</v>
-      </c>
-      <c r="J10" s="16">
-        <v>365</v>
-      </c>
-      <c r="K10" s="16">
-        <v>365</v>
-      </c>
-      <c r="L10" s="16">
-        <v>357</v>
-      </c>
+      <c r="D10" s="16"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="16"/>
+      <c r="L10" s="16"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1249,49 +1233,49 @@
         <v>10</v>
       </c>
       <c r="C12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="D12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="E12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="F12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="G12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="H12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="I12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="J12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="K12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="L12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="M12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="N12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="O12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="P12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
       <c r="Q12" s="16">
-        <v>366.43</v>
+        <v>268.06</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -1300,35 +1284,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="16">
-        <v>38</v>
-      </c>
-      <c r="D13" s="16">
-        <v>42</v>
-      </c>
-      <c r="E13" s="16">
-        <v>42</v>
-      </c>
-      <c r="F13" s="16">
-        <v>40</v>
-      </c>
-      <c r="G13" s="16">
-        <v>35</v>
-      </c>
-      <c r="H13" s="16">
-        <v>39</v>
-      </c>
-      <c r="I13" s="16">
-        <v>35</v>
-      </c>
-      <c r="J13" s="16">
-        <v>35</v>
-      </c>
-      <c r="K13" s="16">
-        <v>33</v>
-      </c>
-      <c r="L13" s="16">
-        <v>29</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D13" s="16"/>
+      <c r="E13" s="16"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="16"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16"/>
     </row>
     <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15"/>
@@ -1342,43 +1308,43 @@
       </c>
       <c r="C15">
         <f t="shared" ref="C15:Q15" si="0">C6*COS(RADIANS(C9-2.83))*C12/1000</f>
-        <v>8.0675396019501164</v>
+        <v>8.9155115680637369</v>
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
-        <v>7.9330519454008748</v>
+        <v>0</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>7.3134098135653147</v>
+        <v>0</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>5.4403868635278192</v>
+        <v>0</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>3.8602595964605353</v>
+        <v>0</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>2.6040170404989795</v>
+        <v>0</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>2.3146705904242482</v>
+        <v>0</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>1.3400292404683321</v>
+        <v>0</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>0.89512949965771826</v>
+        <v>0</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>0.35577898666328733</v>
+        <v>0</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Updated code and added graphs to pinned experiments
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD200211-D52A-4C4D-84E1-943E5D39E2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80F05F1D-0C01-41B1-A9E6-195E27994448}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="9060" windowWidth="29040" windowHeight="15720" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm" sheetId="2" r:id="rId1"/>
     <sheet name="FlxTest10mm" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,8 +24,11 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -315,6 +318,1922 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>ExtTest10mm!$C$7:$K$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-102</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-100</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-81.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-66</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-47</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-17</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-11</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>ExtTest10mm!$C$15:$K$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.9692704311431557</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.7818942292687066</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.9788533640924975</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6672199509713548</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.6232668262422836</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.0879062494581437</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.5793137015132115</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.3116334131211418</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6CE6-48F4-99E2-B8A6EDEFF9C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1196127263"/>
+        <c:axId val="1196114783"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1196127263"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1196114783"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1196114783"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1196127263"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="log"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FlxTest10mm!$C$7:$M$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-24</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-23</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-21</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-35</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-45</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-52</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-61</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-65</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FlxTest10mm!$C$15:$M$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>-13.935059734247528</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-13.417236475994637</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-11.540523984249234</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-9.4436815618485106</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-13.616740654367296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-13.666795063120658</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-8.9358794930124255</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.7882896737922795</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.3535329468122539</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-1.8332483289786352</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-0.53137632724018413</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A9C6-4DEF-A029-39FE8F262D4E}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1394438799"/>
+        <c:axId val="1190584639"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1394438799"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1190584639"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1190584639"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1394438799"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>106362</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>65087</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>676804</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>93662</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9589E56E-6E4D-4018-98E3-3F4B42592F79}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>74083</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>26987</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>331258</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>55562</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4EA82CB5-3533-401A-BE22-19227AB1F59F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -614,28 +2533,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1171875" style="5"/>
+    <col min="2" max="2" width="25.1171875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="5" max="5" width="8.703125" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="13.29296875" customWidth="1"/>
+    <col min="8" max="9" width="13.41015625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -643,7 +2562,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -652,7 +2571,7 @@
         <v>377.65</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -660,7 +2579,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -710,7 +2629,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -742,39 +2661,39 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>102</v>
+        <v>-102</v>
       </c>
       <c r="D7">
-        <v>100</v>
+        <v>-100</v>
       </c>
       <c r="E7">
-        <v>81.5</v>
+        <v>-81.5</v>
       </c>
       <c r="F7">
-        <v>66</v>
+        <v>-66</v>
       </c>
       <c r="G7">
-        <v>47</v>
+        <v>-47</v>
       </c>
       <c r="H7">
-        <v>35</v>
+        <v>-35</v>
       </c>
       <c r="I7">
-        <v>17</v>
+        <v>-17</v>
       </c>
       <c r="J7">
-        <v>11</v>
+        <v>-11</v>
       </c>
       <c r="K7">
-        <v>5</v>
+        <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -814,7 +2733,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -834,7 +2753,7 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -872,7 +2791,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -880,7 +2799,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -928,7 +2847,7 @@
         <v>268.06</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -961,13 +2880,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -1028,7 +2947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.5">
       <c r="G17" t="s">
         <v>18</v>
       </c>
@@ -1036,6 +2955,7 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -1043,28 +2963,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.1171875" style="5"/>
+    <col min="2" max="2" width="19.703125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.29296875" customWidth="1"/>
+    <col min="5" max="5" width="8.703125" customWidth="1"/>
+    <col min="6" max="6" width="11.29296875" customWidth="1"/>
+    <col min="7" max="7" width="13.29296875" customWidth="1"/>
+    <col min="8" max="9" width="13.41015625" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A1" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -1072,7 +2992,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -1081,7 +3001,7 @@
         <v>402.55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
       <c r="G4" t="s">
         <v>19</v>
       </c>
@@ -1089,7 +3009,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.5">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -1139,7 +3059,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -1177,45 +3097,45 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
       <c r="C7">
-        <v>10</v>
+        <v>-10</v>
       </c>
       <c r="D7">
-        <v>14</v>
+        <v>-14</v>
       </c>
       <c r="E7">
-        <v>24</v>
+        <v>-24</v>
       </c>
       <c r="F7">
-        <v>27</v>
+        <v>-27</v>
       </c>
       <c r="G7">
-        <v>23</v>
+        <v>-23</v>
       </c>
       <c r="H7">
-        <v>21</v>
+        <v>-21</v>
       </c>
       <c r="I7">
-        <v>35</v>
+        <v>-35</v>
       </c>
       <c r="J7">
-        <v>45</v>
+        <v>-45</v>
       </c>
       <c r="K7">
-        <v>52</v>
+        <v>-52</v>
       </c>
       <c r="L7">
-        <v>61</v>
+        <v>-61</v>
       </c>
       <c r="M7">
-        <v>65</v>
+        <v>-65</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -1260,7 +3180,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -1281,7 +3201,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -1324,7 +3244,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -1347,7 +3267,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -1398,7 +3318,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1437,59 +3357,59 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.5">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
       <c r="C15">
-        <f>C6*SIN(RADIANS(C8))*C12/1000</f>
-        <v>13.935059734247528</v>
+        <f>C6*-SIN(RADIANS(C8))*C12/1000</f>
+        <v>-13.935059734247528</v>
       </c>
       <c r="D15">
-        <f t="shared" ref="C15:Q15" si="0">D6*COS(RADIANS(D9-2.83))*D12/1000</f>
-        <v>13.433596685970903</v>
+        <f t="shared" ref="D15:O15" si="0">D6*-SIN(RADIANS(D8))*D12/1000</f>
+        <v>-13.417236475994637</v>
       </c>
       <c r="E15">
         <f t="shared" si="0"/>
-        <v>11.579760343306916</v>
+        <v>-11.540523984249234</v>
       </c>
       <c r="F15">
         <f t="shared" si="0"/>
-        <v>9.4841192602954543</v>
+        <v>-9.4436815618485106</v>
       </c>
       <c r="G15">
         <f t="shared" si="0"/>
-        <v>13.702268619690319</v>
+        <v>-13.616740654367296</v>
       </c>
       <c r="H15">
         <f t="shared" si="0"/>
-        <v>13.702268619690319</v>
+        <v>-13.666795063120658</v>
       </c>
       <c r="I15">
         <f t="shared" si="0"/>
-        <v>8.9467753928566189</v>
+        <v>-8.9358794930124255</v>
       </c>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>5.8033137683394296</v>
+        <v>-5.7882896737922795</v>
       </c>
       <c r="K15">
         <f t="shared" si="0"/>
-        <v>3.4121335582366088</v>
+        <v>-3.3535329468122539</v>
       </c>
       <c r="L15">
         <f t="shared" si="0"/>
-        <v>1.8538363426639843</v>
+        <v>-1.8332483289786352</v>
       </c>
       <c r="M15">
         <f t="shared" si="0"/>
-        <v>0.537343867438836</v>
+        <v>-0.53137632724018413</v>
       </c>
       <c r="N15">
         <f t="shared" si="0"/>
@@ -1500,20 +3420,20 @@
         <v>0</v>
       </c>
       <c r="P15">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D15:Q15" si="1">P6*COS(RADIANS(P9-2.83))*P12/1000</f>
         <v>0</v>
       </c>
       <c r="Q15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
       <c r="G16" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.5">
       <c r="H17" t="s">
         <v>22</v>
       </c>
@@ -1521,5 +3441,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Collected data with load cell
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A2FE43-87A0-4073-B21A-755D3289975B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BC590A0-BBA1-4A07-A9A2-069A0F986D72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3105" yWindow="1080" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="1980" yWindow="1515" windowWidth="21600" windowHeight="11385" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="2" r:id="rId1"/>
@@ -8528,7 +8528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B21" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -8958,7 +8958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA6FDC1-BE91-452E-9828-27A0F9CF4E65}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B21" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -9439,7 +9439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50982267-BE91-4E95-AD63-2E538907EFD2}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed spelling errors, made force calculation more accurate
Made force calculation more accurate by taking into account known pressure and maximum BPA contraction %
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E98EB5B6-47CA-4F45-8147-7DBD2EC9BC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA49AA6E-806A-4CBB-830D-4FC64FE23966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-22500" yWindow="1230" windowWidth="21600" windowHeight="11385" firstSheet="2" activeTab="6" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="2" r:id="rId1"/>
@@ -92,9 +92,6 @@
     <t>tendon</t>
   </si>
   <si>
-    <t>Flexsor Test 10mm</t>
-  </si>
-  <si>
     <t>*Fish scale seems to be +/- 1 N</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>****"eccentric"</t>
+  </si>
+  <si>
+    <t>Flexor Test 10mm</t>
   </si>
 </sst>
 </file>
@@ -8528,8 +8528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8554,7 +8554,7 @@
         <v>5</v>
       </c>
       <c r="C2">
-        <v>480</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -8563,7 +8563,7 @@
       </c>
       <c r="C3">
         <f>C2-C2*0.17</f>
-        <v>398.4</v>
+        <v>379.31</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
@@ -8944,7 +8944,7 @@
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -8958,7 +8958,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FA6FDC1-BE91-452E-9828-27A0F9CF4E65}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
@@ -8987,7 +8987,7 @@
         <v>480</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -9425,7 +9425,7 @@
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -9439,8 +9439,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50982267-BE91-4E95-AD63-2E538907EFD2}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9468,7 +9468,7 @@
         <v>480</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:25" x14ac:dyDescent="0.25">
@@ -9488,7 +9488,7 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -10127,12 +10127,12 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.25">
       <c r="N16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -10146,8 +10146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10164,7 +10164,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -10186,10 +10186,10 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -10613,12 +10613,12 @@
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="17" spans="8:8" x14ac:dyDescent="0.25">
       <c r="H17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -10632,8 +10632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6146F73C-E4FC-4324-9793-33EFE048507C}">
   <dimension ref="A1:U15"/>
   <sheetViews>
-    <sheetView topLeftCell="B21" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10650,7 +10650,7 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -10661,7 +10661,7 @@
         <v>455</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
@@ -11259,9 +11259,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D752D96D-CFF4-4F0D-A512-550321C29C07}">
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -11277,7 +11275,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -11288,7 +11286,7 @@
         <v>455</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -11302,10 +11300,10 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="R4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="U4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -12102,17 +12100,17 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="R16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="21:21" x14ac:dyDescent="0.25">
       <c r="U18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -12126,8 +12124,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E5B9E9-F1B4-4DAB-B7CA-9BCB2303132C}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="AG11" sqref="AG11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12144,7 +12142,7 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
@@ -12155,7 +12153,7 @@
         <v>485</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:36" x14ac:dyDescent="0.25">
@@ -12169,22 +12167,22 @@
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="B4" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C4">
         <v>398</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="W4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="AC4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
@@ -13124,25 +13122,25 @@
     </row>
     <row r="16" spans="1:36" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="10:29" x14ac:dyDescent="0.25">
       <c r="J17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="10:29" x14ac:dyDescent="0.25">
       <c r="W18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" spans="10:29" x14ac:dyDescent="0.25">
       <c r="AC19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created pinned knee flexor figures, created Festo Lookup tables
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4DFDE21-1C9A-4095-B13C-F9A14A900745}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40777964-7DE3-4436-A4FB-30BB7BAA4A2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13866" activeTab="6" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="2" r:id="rId1"/>
@@ -10148,8 +10148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -12126,8 +12126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09E5B9E9-F1B4-4DAB-B7CA-9BCB2303132C}">
   <dimension ref="A1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q24" sqref="Q24"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:AG13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>

</xml_diff>

<commit_message>
Updating graphs and data analysis
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A477542-FC7A-4C39-BE22-B000DBA204C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{379E4E0C-56DF-45DE-AAED-2F7BCC24CDE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25425" yWindow="1875" windowWidth="13455" windowHeight="11385" firstSheet="2" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="FlxTest10mm_3" sheetId="6" r:id="rId6"/>
     <sheet name="FlxTest10mm_4" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -8570,28 +8572,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="25.15625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -8599,7 +8601,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -8608,7 +8610,7 @@
         <v>379.31</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -8616,7 +8618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -8666,7 +8668,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -8698,7 +8700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -8730,7 +8732,7 @@
         <v>-5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -8770,7 +8772,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -8790,7 +8792,7 @@
       <c r="O9" s="16"/>
       <c r="P9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -8828,7 +8830,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -8836,7 +8838,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -8884,7 +8886,7 @@
         <v>268.06</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -8917,13 +8919,13 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -8984,7 +8986,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" t="s">
         <v>17</v>
       </c>
@@ -9001,27 +9003,27 @@
   <dimension ref="A1:Q17"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="25.15625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -9032,7 +9034,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -9041,7 +9043,7 @@
         <v>398.4</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -9049,7 +9051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -9099,7 +9101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -9143,7 +9145,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -9187,7 +9189,7 @@
         <v>-113.5</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -9234,7 +9236,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -9245,7 +9247,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -9290,7 +9292,7 @@
         <v>443.5</v>
       </c>
     </row>
-    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -9298,7 +9300,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -9349,7 +9351,7 @@
         <v>268.06</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -9394,13 +9396,13 @@
         <v>55.5</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -9465,7 +9467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" t="s">
         <v>17</v>
       </c>
@@ -9481,28 +9483,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50982267-BE91-4E95-AD63-2E538907EFD2}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="25.140625" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="25.15625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -9513,7 +9515,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -9522,7 +9524,7 @@
         <v>398.4</v>
       </c>
     </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5" t="s">
         <v>16</v>
       </c>
@@ -9533,7 +9535,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:25" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -9607,7 +9609,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -9678,7 +9680,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -9749,7 +9751,7 @@
         <v>-107</v>
       </c>
     </row>
-    <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -9823,7 +9825,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="9" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:25" s="17" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -9834,7 +9836,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -9906,7 +9908,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:25" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -9914,7 +9916,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="18"/>
       <c r="B12" s="19" t="s">
         <v>10</v>
@@ -9989,7 +9991,7 @@
         <v>268.06</v>
       </c>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -10064,13 +10066,13 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:25" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -10167,12 +10169,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.55000000000000004">
       <c r="N16" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" t="s">
         <v>17</v>
       </c>
@@ -10188,28 +10190,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55F358BD-411F-4156-AA93-0DF96BD5C242}">
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="19.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -10217,7 +10219,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -10226,7 +10228,7 @@
         <v>402.55</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -10234,7 +10236,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -10284,7 +10286,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -10322,7 +10324,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -10360,7 +10362,7 @@
         <v>-65</v>
       </c>
     </row>
-    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -10405,7 +10407,7 @@
       <c r="P8" s="4"/>
       <c r="Q8" s="4"/>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -10426,7 +10428,7 @@
       <c r="P9" s="16"/>
       <c r="Q9" s="16"/>
     </row>
-    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -10469,7 +10471,7 @@
       <c r="P10" s="1"/>
       <c r="Q10" s="1"/>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -10492,7 +10494,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -10543,7 +10545,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -10582,13 +10584,13 @@
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -10653,12 +10655,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.55000000000000004">
       <c r="G16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="H17" t="s">
         <v>21</v>
       </c>
@@ -10666,17 +10668,17 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L22" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L24" t="s">
         <v>42</v>
       </c>
@@ -10687,7 +10689,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="25" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L25">
         <v>0</v>
       </c>
@@ -10698,7 +10700,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L26">
         <v>45</v>
       </c>
@@ -10709,17 +10711,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="30" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L30" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="31" spans="8:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="8:14" x14ac:dyDescent="0.55000000000000004">
       <c r="L31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="12:12" x14ac:dyDescent="0.55000000000000004">
       <c r="L33" t="s">
         <v>50</v>
       </c>
@@ -10739,24 +10741,24 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="19.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -10767,7 +10769,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>37</v>
       </c>
@@ -10778,7 +10780,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -10845,7 +10847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -10904,7 +10906,7 @@
         <v>69.599999999999994</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -10963,7 +10965,7 @@
         <v>-23</v>
       </c>
     </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -11026,7 +11028,7 @@
       </c>
       <c r="U8" s="4"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -11051,7 +11053,7 @@
       <c r="T9" s="16"/>
       <c r="U9" s="16"/>
     </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -11112,7 +11114,7 @@
       </c>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -11139,7 +11141,7 @@
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -11206,7 +11208,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -11266,13 +11268,13 @@
         <v>79.5</v>
       </c>
     </row>
-    <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -11364,26 +11366,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D752D96D-CFF4-4F0D-A512-550321C29C07}">
   <dimension ref="A1:AJ18"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0"/>
+    <sheetView topLeftCell="J1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="19.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -11394,7 +11396,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -11403,7 +11405,7 @@
         <v>377.65</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="R4" t="s">
         <v>18</v>
       </c>
@@ -11411,7 +11413,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -11506,7 +11508,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -11589,7 +11591,7 @@
         <v>72.5</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -11672,7 +11674,7 @@
         <v>-26.5</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -11758,7 +11760,7 @@
         <v>82.5</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -11798,7 +11800,7 @@
       <c r="AI9" s="17"/>
       <c r="AJ9" s="17"/>
     </row>
-    <row r="10" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -11890,7 +11892,7 @@
       <c r="AI10" s="17"/>
       <c r="AJ10" s="17"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -11916,7 +11918,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -12004,7 +12006,7 @@
       <c r="AE12" s="16"/>
       <c r="AF12" s="16"/>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -12088,13 +12090,13 @@
         <v>85</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -12203,17 +12205,17 @@
         <v>-19.335653408942736</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="R16" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="17" spans="21:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U17" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="21:21" x14ac:dyDescent="0.25">
+    <row r="18" spans="21:21" x14ac:dyDescent="0.55000000000000004">
       <c r="U18" t="s">
         <v>26</v>
       </c>
@@ -12230,27 +12232,27 @@
   <dimension ref="A1:AJ19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13:AG13"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="5"/>
-    <col min="2" max="2" width="19.7109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="8.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
-    <col min="8" max="9" width="13.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.15625" style="5"/>
+    <col min="2" max="2" width="19.68359375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="12.26171875" customWidth="1"/>
+    <col min="5" max="5" width="8.68359375" customWidth="1"/>
+    <col min="6" max="6" width="11.26171875" customWidth="1"/>
+    <col min="7" max="7" width="13.26171875" customWidth="1"/>
+    <col min="8" max="9" width="13.41796875" customWidth="1"/>
     <col min="10" max="10" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>5</v>
       </c>
@@ -12261,7 +12263,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" s="5" t="s">
         <v>14</v>
       </c>
@@ -12270,7 +12272,7 @@
         <v>402.55</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" s="5" t="s">
         <v>31</v>
       </c>
@@ -12290,7 +12292,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:36" s="12" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
@@ -12413,7 +12415,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
@@ -12511,7 +12513,7 @@
         <v>62.7</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -12609,7 +12611,7 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
@@ -12710,7 +12712,7 @@
         <v>103.5</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="14"/>
       <c r="B9" s="10" t="s">
         <v>13</v>
@@ -12750,7 +12752,7 @@
       <c r="AI9" s="17"/>
       <c r="AJ9" s="17"/>
     </row>
-    <row r="10" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="14"/>
       <c r="B10" s="10" t="s">
         <v>3</v>
@@ -12852,7 +12854,7 @@
       <c r="AI10" s="3"/>
       <c r="AJ10" s="3"/>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="13" t="s">
         <v>8</v>
       </c>
@@ -12878,7 +12880,7 @@
       <c r="S11" s="2"/>
       <c r="T11" s="2"/>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="14"/>
       <c r="B12" s="10" t="s">
         <v>10</v>
@@ -12983,7 +12985,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="14"/>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -13082,13 +13084,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="14" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:36" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="15"/>
       <c r="B14" s="11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>6</v>
       </c>
@@ -13225,12 +13227,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.55000000000000004">
       <c r="J16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="10:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:29" x14ac:dyDescent="0.55000000000000004">
       <c r="J17" t="s">
         <v>30</v>
       </c>
@@ -13238,12 +13240,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="10:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:29" x14ac:dyDescent="0.55000000000000004">
       <c r="W18" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="10:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:29" x14ac:dyDescent="0.55000000000000004">
       <c r="AC19" t="s">
         <v>35</v>
       </c>

</xml_diff>

<commit_message>
More figures, added fits
Added fit figures for f20 and f40. Normalized f20 and f40. Now when calling them use relative strain and relative pressure. Festo4 updated to calculate this. Created a figure for Ext10mm_group, even though 41.5cm results aren't optimized. Removed old ExtPin_10mm figures and files. MonoPamDataExplicit is updated to be like MonoPamDataExplicit_compare except to only call for force calculations using the simplified exponential equation.
</commit_message>
<xml_diff>
--- a/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
+++ b/Testing_Data/2022_02_Festo/Results_table_10mm_pinned_FishScale.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ben\Documents\GitHub\Bipedal_Robot\Testing_Data\2022_02_Festo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2465B52-41D4-482E-8E18-B612FF1267D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72354B7-638F-48A1-A884-E76578A00617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
+    <workbookView xWindow="29820" yWindow="3195" windowWidth="21630" windowHeight="11250" activeTab="2" xr2:uid="{FDAF32CB-2BA8-47E2-927E-3C1E6066A0C3}"/>
   </bookViews>
   <sheets>
     <sheet name="ExtTest10mm_1" sheetId="2" r:id="rId1"/>
@@ -8662,7 +8662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DDD6FA0-ED90-4B9F-A1DF-3E2DAEF07409}">
   <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
@@ -9544,7 +9544,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50982267-BE91-4E95-AD63-2E538907EFD2}">
   <dimension ref="A1:Y17"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
@@ -10247,7 +10247,7 @@
   <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>